<commit_message>
added obj value; updated datasets
</commit_message>
<xml_diff>
--- a/DataSets/Calumpit shelter data.xlsx
+++ b/DataSets/Calumpit shelter data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PERSONAL\BRYAN\bulsu\Thesis 1\ShelterAlloc_Thesis\DataSets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34273B80-3E14-4557-91ED-58C902CDEAF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1456613-3E84-456D-A675-F3F1E8EA6FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="47">
   <si>
     <t>Remarks</t>
   </si>
@@ -163,6 +163,15 @@
   </si>
   <si>
     <t>Empty Lot</t>
+  </si>
+  <si>
+    <t>Iba O'Este Empty Lot 3</t>
+  </si>
+  <si>
+    <t>Iba O'Este Empty Lot 4</t>
+  </si>
+  <si>
+    <t>Caniogan Empty Lot 2</t>
   </si>
 </sst>
 </file>
@@ -482,7 +491,7 @@
   <dimension ref="A1:W999"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1489,7 +1498,7 @@
     </row>
     <row r="29" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B29" s="5">
         <v>14.906123709999999</v>
@@ -1524,7 +1533,7 @@
     </row>
     <row r="30" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B30" s="5">
         <v>14.9074852</v>
@@ -1559,7 +1568,7 @@
     </row>
     <row r="31" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B31" s="5">
         <v>14.907812399999999</v>

</xml_diff>